<commit_message>
Practiced Formatting & Groupby
</commit_message>
<xml_diff>
--- a/formatting.xlsx
+++ b/formatting.xlsx
@@ -8,18 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WolfCoder\Desktop\ds_prac\excel-for-datascience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B085A1BE-8D01-4320-B01E-D1DBC4F6FC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAD3DB2-1D3D-483C-BD50-D326970D558F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Formatting" sheetId="2" r:id="rId1"/>
     <sheet name="Original" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -79,7 +90,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00,&quot;K&quot;"/>
-    <numFmt numFmtId="167" formatCode="dd/dddd/mmm/yy"/>
+    <numFmt numFmtId="165" formatCode="dd/dddd/mmm/yy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -130,8 +141,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -508,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A009C0B4-F6CA-43E6-B6C1-BE6269649279}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>